<commit_message>
AIP-1584 AIP-1587 Updated test data and mds file
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_16Channel/1U1U3I3I.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/CablingDataSet/CablingDataSet_16Channel/1U1U3I3I.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CD3F87-C12B-4D5E-B640-B6ACA35BC36D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1937BC44-D810-4B97-BE06-6EFD9F387317}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1513,6 +1513,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">

</xml_diff>